<commit_message>
Assingment 2 Stack and Queue : Exception Handling
</commit_message>
<xml_diff>
--- a/dsa/DSA_Assingment2/allocatedCandidates.xlsx
+++ b/dsa/DSA_Assingment2/allocatedCandidates.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="312">
   <si>
     <t>Student name</t>
   </si>
@@ -29,82 +29,82 @@
     <t>Name2</t>
   </si>
   <si>
+    <t>IT2</t>
+  </si>
+  <si>
     <t>Name3</t>
   </si>
   <si>
-    <t>IT2</t>
-  </si>
-  <si>
     <t>Name4</t>
   </si>
   <si>
+    <t>IT4</t>
+  </si>
+  <si>
+    <t>Name5</t>
+  </si>
+  <si>
+    <t>IT5</t>
+  </si>
+  <si>
+    <t>Name6</t>
+  </si>
+  <si>
+    <t>Name7</t>
+  </si>
+  <si>
+    <t>IT7</t>
+  </si>
+  <si>
+    <t>Name8</t>
+  </si>
+  <si>
+    <t>Name9</t>
+  </si>
+  <si>
+    <t>IT9</t>
+  </si>
+  <si>
+    <t>Name10</t>
+  </si>
+  <si>
+    <t>Name11</t>
+  </si>
+  <si>
+    <t>IT10</t>
+  </si>
+  <si>
+    <t>Name12</t>
+  </si>
+  <si>
+    <t>Name13</t>
+  </si>
+  <si>
+    <t>Name14</t>
+  </si>
+  <si>
     <t>IT3</t>
   </si>
   <si>
-    <t>Name5</t>
-  </si>
-  <si>
-    <t>IT5</t>
-  </si>
-  <si>
-    <t>Name6</t>
-  </si>
-  <si>
-    <t>Name7</t>
+    <t>Name15</t>
+  </si>
+  <si>
+    <t>Name16</t>
+  </si>
+  <si>
+    <t>Name17</t>
   </si>
   <si>
     <t>IT6</t>
   </si>
   <si>
-    <t>Name8</t>
+    <t>Name18</t>
+  </si>
+  <si>
+    <t>Name19</t>
   </si>
   <si>
     <t>IT8</t>
-  </si>
-  <si>
-    <t>Name9</t>
-  </si>
-  <si>
-    <t>IT9</t>
-  </si>
-  <si>
-    <t>Name10</t>
-  </si>
-  <si>
-    <t>Name11</t>
-  </si>
-  <si>
-    <t>IT10</t>
-  </si>
-  <si>
-    <t>Name12</t>
-  </si>
-  <si>
-    <t>Name13</t>
-  </si>
-  <si>
-    <t>Name14</t>
-  </si>
-  <si>
-    <t>Name15</t>
-  </si>
-  <si>
-    <t>IT4</t>
-  </si>
-  <si>
-    <t>Name16</t>
-  </si>
-  <si>
-    <t>Name17</t>
-  </si>
-  <si>
-    <t>Name18</t>
-  </si>
-  <si>
-    <t>IT7</t>
-  </si>
-  <si>
-    <t>Name19</t>
   </si>
   <si>
     <t>Name20</t>
@@ -1019,15 +1019,15 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -1067,36 +1067,36 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -1123,23 +1123,23 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -1147,15 +1147,15 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
         <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="21">
@@ -1163,7 +1163,7 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -1171,7 +1171,7 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23">
@@ -1179,21 +1179,23 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -1201,7 +1203,7 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
@@ -1209,7 +1211,7 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28">
@@ -1217,7 +1219,7 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
@@ -1225,7 +1227,7 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
@@ -1241,7 +1243,7 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32">
@@ -1249,7 +1251,7 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33">
@@ -1257,7 +1259,7 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34">
@@ -1265,21 +1267,23 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
         <v>45</v>
       </c>
-      <c r="B35"/>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1287,7 +1291,7 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1295,7 +1299,7 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39">
@@ -1303,7 +1307,7 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1311,7 +1315,7 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41">
@@ -1327,7 +1331,7 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43">
@@ -1335,7 +1339,7 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44">
@@ -1343,7 +1347,7 @@
         <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45">
@@ -1351,21 +1355,23 @@
         <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
         <v>56</v>
       </c>
-      <c r="B46"/>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
         <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1373,7 +1379,7 @@
         <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
@@ -1381,7 +1387,7 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50">
@@ -1397,7 +1403,7 @@
         <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
@@ -1405,7 +1411,7 @@
         <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53">
@@ -1413,7 +1419,7 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54">
@@ -1421,7 +1427,7 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55">
@@ -1429,7 +1435,7 @@
         <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56">
@@ -1437,21 +1443,23 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
         <v>67</v>
       </c>
-      <c r="B57"/>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
         <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -1459,7 +1467,7 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
@@ -1467,7 +1475,7 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61">
@@ -1483,7 +1491,7 @@
         <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63">
@@ -1499,7 +1507,7 @@
         <v>74</v>
       </c>
       <c r="B64" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65">
@@ -1507,7 +1515,7 @@
         <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66">
@@ -1515,7 +1523,7 @@
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67">
@@ -1523,21 +1531,23 @@
         <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
         <v>78</v>
       </c>
-      <c r="B68"/>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
         <v>79</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1545,7 +1555,7 @@
         <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71">
@@ -1553,7 +1563,7 @@
         <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72">
@@ -1561,7 +1571,7 @@
         <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73">
@@ -1585,7 +1595,7 @@
         <v>85</v>
       </c>
       <c r="B75" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76">
@@ -1593,7 +1603,7 @@
         <v>86</v>
       </c>
       <c r="B76" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77">
@@ -1601,7 +1611,7 @@
         <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78">
@@ -1609,21 +1619,23 @@
         <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
         <v>89</v>
       </c>
-      <c r="B79"/>
+      <c r="B79" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
         <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -1631,7 +1643,7 @@
         <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -1639,7 +1651,7 @@
         <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83">
@@ -1655,7 +1667,7 @@
         <v>94</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85">
@@ -1671,7 +1683,7 @@
         <v>96</v>
       </c>
       <c r="B86" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87">
@@ -1679,7 +1691,7 @@
         <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88">
@@ -1687,7 +1699,7 @@
         <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89">
@@ -1695,21 +1707,23 @@
         <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
         <v>100</v>
       </c>
-      <c r="B90"/>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
         <v>101</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92">
@@ -1717,7 +1731,7 @@
         <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
@@ -1725,7 +1739,7 @@
         <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94">
@@ -1741,7 +1755,7 @@
         <v>105</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96">
@@ -1757,7 +1771,7 @@
         <v>107</v>
       </c>
       <c r="B97" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98">
@@ -1765,7 +1779,7 @@
         <v>108</v>
       </c>
       <c r="B98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99">
@@ -1773,7 +1787,7 @@
         <v>109</v>
       </c>
       <c r="B99" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100">
@@ -1781,21 +1795,23 @@
         <v>110</v>
       </c>
       <c r="B100" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
         <v>111</v>
       </c>
-      <c r="B101"/>
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
         <v>112</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -1803,7 +1819,7 @@
         <v>113</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="104">
@@ -1811,7 +1827,7 @@
         <v>114</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105">
@@ -1819,7 +1835,7 @@
         <v>115</v>
       </c>
       <c r="B105" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106">
@@ -1827,7 +1843,7 @@
         <v>116</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107">
@@ -1843,7 +1859,7 @@
         <v>118</v>
       </c>
       <c r="B108" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109">
@@ -1851,7 +1867,7 @@
         <v>119</v>
       </c>
       <c r="B109" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110">
@@ -1859,7 +1875,7 @@
         <v>120</v>
       </c>
       <c r="B110" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="111">
@@ -1867,21 +1883,23 @@
         <v>121</v>
       </c>
       <c r="B111" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
         <v>122</v>
       </c>
-      <c r="B112"/>
+      <c r="B112" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
         <v>123</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114">
@@ -1889,7 +1907,7 @@
         <v>124</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115">
@@ -1905,7 +1923,7 @@
         <v>126</v>
       </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117">
@@ -1913,23 +1931,21 @@
         <v>127</v>
       </c>
       <c r="B117" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
         <v>128</v>
       </c>
-      <c r="B118" t="s">
-        <v>13</v>
-      </c>
+      <c r="B118"/>
     </row>
     <row r="119">
       <c r="A119" t="s">
         <v>129</v>
       </c>
       <c r="B119" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="120">
@@ -1937,7 +1953,7 @@
         <v>130</v>
       </c>
       <c r="B120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121">
@@ -1945,7 +1961,7 @@
         <v>131</v>
       </c>
       <c r="B121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122">
@@ -1953,21 +1969,23 @@
         <v>132</v>
       </c>
       <c r="B122" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
         <v>133</v>
       </c>
-      <c r="B123"/>
+      <c r="B123" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
         <v>134</v>
       </c>
       <c r="B124" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
@@ -1975,7 +1993,7 @@
         <v>135</v>
       </c>
       <c r="B125" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126">
@@ -1991,7 +2009,7 @@
         <v>137</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128">
@@ -1999,23 +2017,21 @@
         <v>138</v>
       </c>
       <c r="B128" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
         <v>139</v>
       </c>
-      <c r="B129" t="s">
-        <v>13</v>
-      </c>
+      <c r="B129"/>
     </row>
     <row r="130">
       <c r="A130" t="s">
         <v>140</v>
       </c>
       <c r="B130" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="131">
@@ -2023,7 +2039,7 @@
         <v>141</v>
       </c>
       <c r="B131" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="132">
@@ -2031,7 +2047,7 @@
         <v>142</v>
       </c>
       <c r="B132" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="133">
@@ -2039,21 +2055,23 @@
         <v>143</v>
       </c>
       <c r="B133" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
         <v>144</v>
       </c>
-      <c r="B134"/>
+      <c r="B134" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
         <v>145</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136">
@@ -2061,7 +2079,7 @@
         <v>146</v>
       </c>
       <c r="B136" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137">
@@ -2077,7 +2095,7 @@
         <v>148</v>
       </c>
       <c r="B138" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139">
@@ -2085,23 +2103,21 @@
         <v>149</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
         <v>150</v>
       </c>
-      <c r="B140" t="s">
-        <v>13</v>
-      </c>
+      <c r="B140"/>
     </row>
     <row r="141">
       <c r="A141" t="s">
         <v>151</v>
       </c>
       <c r="B141" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="142">
@@ -2109,7 +2125,7 @@
         <v>152</v>
       </c>
       <c r="B142" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="143">
@@ -2117,7 +2133,7 @@
         <v>153</v>
       </c>
       <c r="B143" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144">
@@ -2125,27 +2141,31 @@
         <v>154</v>
       </c>
       <c r="B144" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
         <v>155</v>
       </c>
-      <c r="B145"/>
+      <c r="B145" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
         <v>156</v>
       </c>
-      <c r="B146"/>
+      <c r="B146" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
         <v>157</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="148">
@@ -2153,7 +2173,7 @@
         <v>158</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149">
@@ -2161,7 +2181,7 @@
         <v>159</v>
       </c>
       <c r="B149" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150">
@@ -2169,23 +2189,21 @@
         <v>160</v>
       </c>
       <c r="B150" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
         <v>161</v>
       </c>
-      <c r="B151" t="s">
-        <v>13</v>
-      </c>
+      <c r="B151"/>
     </row>
     <row r="152">
       <c r="A152" t="s">
         <v>162</v>
       </c>
       <c r="B152" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153">
@@ -2193,7 +2211,7 @@
         <v>163</v>
       </c>
       <c r="B153" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="154">
@@ -2201,7 +2219,7 @@
         <v>164</v>
       </c>
       <c r="B154" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="155">
@@ -2209,21 +2227,23 @@
         <v>165</v>
       </c>
       <c r="B155" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
         <v>166</v>
       </c>
-      <c r="B156"/>
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
         <v>167</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158">
@@ -2231,7 +2251,7 @@
         <v>168</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="159">
@@ -2239,7 +2259,7 @@
         <v>169</v>
       </c>
       <c r="B159" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="160">
@@ -2247,7 +2267,7 @@
         <v>170</v>
       </c>
       <c r="B160" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="161">
@@ -2255,23 +2275,21 @@
         <v>171</v>
       </c>
       <c r="B161" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
         <v>172</v>
       </c>
-      <c r="B162" t="s">
-        <v>13</v>
-      </c>
+      <c r="B162"/>
     </row>
     <row r="163">
       <c r="A163" t="s">
         <v>173</v>
       </c>
       <c r="B163" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="164">
@@ -2279,7 +2297,7 @@
         <v>174</v>
       </c>
       <c r="B164" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="165">
@@ -2287,7 +2305,7 @@
         <v>175</v>
       </c>
       <c r="B165" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="166">
@@ -2295,21 +2313,23 @@
         <v>176</v>
       </c>
       <c r="B166" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
         <v>177</v>
       </c>
-      <c r="B167"/>
+      <c r="B167" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
         <v>178</v>
       </c>
       <c r="B168" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169">
@@ -2317,7 +2337,7 @@
         <v>179</v>
       </c>
       <c r="B169" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="170">
@@ -2325,7 +2345,7 @@
         <v>180</v>
       </c>
       <c r="B170" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="171">
@@ -2333,7 +2353,7 @@
         <v>181</v>
       </c>
       <c r="B171" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="172">
@@ -2341,23 +2361,21 @@
         <v>182</v>
       </c>
       <c r="B172" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
         <v>183</v>
       </c>
-      <c r="B173" t="s">
-        <v>13</v>
-      </c>
+      <c r="B173"/>
     </row>
     <row r="174">
       <c r="A174" t="s">
         <v>184</v>
       </c>
       <c r="B174" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="175">
@@ -2365,7 +2383,7 @@
         <v>185</v>
       </c>
       <c r="B175" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="176">
@@ -2373,7 +2391,7 @@
         <v>186</v>
       </c>
       <c r="B176" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="177">
@@ -2381,21 +2399,23 @@
         <v>187</v>
       </c>
       <c r="B177" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
         <v>188</v>
       </c>
-      <c r="B178"/>
+      <c r="B178" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
         <v>189</v>
       </c>
       <c r="B179" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
@@ -2403,7 +2423,7 @@
         <v>190</v>
       </c>
       <c r="B180" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="181">
@@ -2411,7 +2431,7 @@
         <v>191</v>
       </c>
       <c r="B181" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="182">
@@ -2419,7 +2439,7 @@
         <v>192</v>
       </c>
       <c r="B182" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183">
@@ -2427,23 +2447,21 @@
         <v>193</v>
       </c>
       <c r="B183" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
         <v>194</v>
       </c>
-      <c r="B184" t="s">
-        <v>13</v>
-      </c>
+      <c r="B184"/>
     </row>
     <row r="185">
       <c r="A185" t="s">
         <v>195</v>
       </c>
       <c r="B185" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="186">
@@ -2451,7 +2469,7 @@
         <v>196</v>
       </c>
       <c r="B186" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="187">
@@ -2459,7 +2477,7 @@
         <v>197</v>
       </c>
       <c r="B187" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="188">
@@ -2467,21 +2485,23 @@
         <v>198</v>
       </c>
       <c r="B188" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
         <v>199</v>
       </c>
-      <c r="B189"/>
+      <c r="B189" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
         <v>200</v>
       </c>
       <c r="B190" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="191">
@@ -2489,7 +2509,7 @@
         <v>201</v>
       </c>
       <c r="B191" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="192">
@@ -2497,7 +2517,7 @@
         <v>202</v>
       </c>
       <c r="B192" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="193">
@@ -2505,7 +2525,7 @@
         <v>203</v>
       </c>
       <c r="B193" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194">
@@ -2513,23 +2533,21 @@
         <v>204</v>
       </c>
       <c r="B194" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="s">
         <v>205</v>
       </c>
-      <c r="B195" t="s">
-        <v>13</v>
-      </c>
+      <c r="B195"/>
     </row>
     <row r="196">
       <c r="A196" t="s">
         <v>206</v>
       </c>
       <c r="B196" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="197">
@@ -2537,7 +2555,7 @@
         <v>207</v>
       </c>
       <c r="B197" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="198">
@@ -2545,7 +2563,7 @@
         <v>208</v>
       </c>
       <c r="B198" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="199">
@@ -2553,21 +2571,23 @@
         <v>209</v>
       </c>
       <c r="B199" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
         <v>210</v>
       </c>
-      <c r="B200"/>
+      <c r="B200" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
         <v>211</v>
       </c>
       <c r="B201" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202">
@@ -2575,7 +2595,7 @@
         <v>212</v>
       </c>
       <c r="B202" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="203">
@@ -2591,7 +2611,7 @@
         <v>214</v>
       </c>
       <c r="B204" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="205">
@@ -2599,23 +2619,21 @@
         <v>215</v>
       </c>
       <c r="B205" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
         <v>216</v>
       </c>
-      <c r="B206" t="s">
-        <v>13</v>
-      </c>
+      <c r="B206"/>
     </row>
     <row r="207">
       <c r="A207" t="s">
         <v>217</v>
       </c>
       <c r="B207" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="208">
@@ -2623,33 +2641,39 @@
         <v>218</v>
       </c>
       <c r="B208" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
         <v>219</v>
       </c>
-      <c r="B209"/>
+      <c r="B209" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
         <v>220</v>
       </c>
-      <c r="B210"/>
+      <c r="B210" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
         <v>221</v>
       </c>
-      <c r="B211"/>
+      <c r="B211" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
         <v>222</v>
       </c>
       <c r="B212" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213">
@@ -2657,7 +2681,7 @@
         <v>223</v>
       </c>
       <c r="B213" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="214">
@@ -2673,7 +2697,7 @@
         <v>225</v>
       </c>
       <c r="B215" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="216">
@@ -2681,23 +2705,21 @@
         <v>226</v>
       </c>
       <c r="B216" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
         <v>227</v>
       </c>
-      <c r="B217" t="s">
-        <v>13</v>
-      </c>
+      <c r="B217"/>
     </row>
     <row r="218">
       <c r="A218" t="s">
         <v>228</v>
       </c>
       <c r="B218" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="219">
@@ -2705,7 +2727,7 @@
         <v>229</v>
       </c>
       <c r="B219" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="220">
@@ -2713,27 +2735,31 @@
         <v>230</v>
       </c>
       <c r="B220" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="s">
         <v>231</v>
       </c>
-      <c r="B221"/>
+      <c r="B221" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="s">
         <v>232</v>
       </c>
-      <c r="B222"/>
+      <c r="B222" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
         <v>233</v>
       </c>
       <c r="B223" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="224">
@@ -2741,7 +2767,7 @@
         <v>234</v>
       </c>
       <c r="B224" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="225">
@@ -2749,7 +2775,7 @@
         <v>235</v>
       </c>
       <c r="B225" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="226">
@@ -2757,7 +2783,7 @@
         <v>236</v>
       </c>
       <c r="B226" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="227">
@@ -2765,7 +2791,7 @@
         <v>237</v>
       </c>
       <c r="B227" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="228">
@@ -2779,7 +2805,7 @@
         <v>239</v>
       </c>
       <c r="B229" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="230">
@@ -2787,7 +2813,7 @@
         <v>240</v>
       </c>
       <c r="B230" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="231">
@@ -2795,27 +2821,31 @@
         <v>241</v>
       </c>
       <c r="B231" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
         <v>242</v>
       </c>
-      <c r="B232"/>
+      <c r="B232" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
         <v>243</v>
       </c>
-      <c r="B233"/>
+      <c r="B233" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
         <v>244</v>
       </c>
       <c r="B234" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="235">
@@ -2823,7 +2853,7 @@
         <v>245</v>
       </c>
       <c r="B235" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="236">
@@ -2831,7 +2861,7 @@
         <v>246</v>
       </c>
       <c r="B236" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="237">
@@ -2839,7 +2869,7 @@
         <v>247</v>
       </c>
       <c r="B237" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="238">
@@ -2847,23 +2877,21 @@
         <v>248</v>
       </c>
       <c r="B238" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
         <v>249</v>
       </c>
-      <c r="B239" t="s">
-        <v>13</v>
-      </c>
+      <c r="B239"/>
     </row>
     <row r="240">
       <c r="A240" t="s">
         <v>250</v>
       </c>
       <c r="B240" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="241">
@@ -2871,7 +2899,7 @@
         <v>251</v>
       </c>
       <c r="B241" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="242">
@@ -2879,27 +2907,31 @@
         <v>252</v>
       </c>
       <c r="B242" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
         <v>253</v>
       </c>
-      <c r="B243"/>
+      <c r="B243" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
         <v>254</v>
       </c>
-      <c r="B244"/>
+      <c r="B244" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
         <v>255</v>
       </c>
       <c r="B245" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="246">
@@ -2907,7 +2939,7 @@
         <v>256</v>
       </c>
       <c r="B246" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="247">
@@ -2915,7 +2947,7 @@
         <v>257</v>
       </c>
       <c r="B247" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="248">
@@ -2923,7 +2955,7 @@
         <v>258</v>
       </c>
       <c r="B248" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249">
@@ -2931,29 +2963,29 @@
         <v>259</v>
       </c>
       <c r="B249" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="s">
         <v>260</v>
       </c>
-      <c r="B250" t="s">
-        <v>13</v>
-      </c>
+      <c r="B250"/>
     </row>
     <row r="251">
       <c r="A251" t="s">
         <v>261</v>
       </c>
-      <c r="B251"/>
+      <c r="B251" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
         <v>262</v>
       </c>
       <c r="B252" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="253">
@@ -2961,14 +2993,16 @@
         <v>263</v>
       </c>
       <c r="B253" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
         <v>264</v>
       </c>
-      <c r="B254"/>
+      <c r="B254" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
@@ -2981,7 +3015,7 @@
         <v>266</v>
       </c>
       <c r="B256" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="257">
@@ -2989,7 +3023,7 @@
         <v>267</v>
       </c>
       <c r="B257" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="258">
@@ -2997,7 +3031,7 @@
         <v>268</v>
       </c>
       <c r="B258" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="259">
@@ -3005,7 +3039,7 @@
         <v>269</v>
       </c>
       <c r="B259" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260">
@@ -3013,16 +3047,14 @@
         <v>270</v>
       </c>
       <c r="B260" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
         <v>271</v>
       </c>
-      <c r="B261" t="s">
-        <v>13</v>
-      </c>
+      <c r="B261"/>
     </row>
     <row r="262">
       <c r="A262" t="s">
@@ -3035,7 +3067,7 @@
         <v>273</v>
       </c>
       <c r="B263" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="264">
@@ -3043,27 +3075,31 @@
         <v>274</v>
       </c>
       <c r="B264" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s">
         <v>275</v>
       </c>
-      <c r="B265"/>
+      <c r="B265" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="s">
         <v>276</v>
       </c>
-      <c r="B266"/>
+      <c r="B266" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
         <v>277</v>
       </c>
       <c r="B267" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="268">
@@ -3071,7 +3107,7 @@
         <v>278</v>
       </c>
       <c r="B268" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="269">
@@ -3079,7 +3115,7 @@
         <v>279</v>
       </c>
       <c r="B269" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="270">
@@ -3087,7 +3123,7 @@
         <v>280</v>
       </c>
       <c r="B270" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="271">
@@ -3095,16 +3131,14 @@
         <v>281</v>
       </c>
       <c r="B271" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="s">
         <v>282</v>
       </c>
-      <c r="B272" t="s">
-        <v>13</v>
-      </c>
+      <c r="B272"/>
     </row>
     <row r="273">
       <c r="A273" t="s">
@@ -3117,7 +3151,7 @@
         <v>284</v>
       </c>
       <c r="B274" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="275">
@@ -3125,27 +3159,31 @@
         <v>285</v>
       </c>
       <c r="B275" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
         <v>286</v>
       </c>
-      <c r="B276"/>
+      <c r="B276" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
         <v>287</v>
       </c>
-      <c r="B277"/>
+      <c r="B277" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
         <v>288</v>
       </c>
       <c r="B278" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="279">
@@ -3153,7 +3191,7 @@
         <v>289</v>
       </c>
       <c r="B279" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="280">
@@ -3161,7 +3199,7 @@
         <v>290</v>
       </c>
       <c r="B280" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="281">
@@ -3169,7 +3207,7 @@
         <v>291</v>
       </c>
       <c r="B281" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282">
@@ -3177,16 +3215,14 @@
         <v>292</v>
       </c>
       <c r="B282" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
         <v>293</v>
       </c>
-      <c r="B283" t="s">
-        <v>13</v>
-      </c>
+      <c r="B283"/>
     </row>
     <row r="284">
       <c r="A284" t="s">
@@ -3199,7 +3235,7 @@
         <v>295</v>
       </c>
       <c r="B285" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="286">
@@ -3207,27 +3243,31 @@
         <v>296</v>
       </c>
       <c r="B286" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s">
         <v>297</v>
       </c>
-      <c r="B287"/>
+      <c r="B287" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="s">
         <v>298</v>
       </c>
-      <c r="B288"/>
+      <c r="B288" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="s">
         <v>299</v>
       </c>
       <c r="B289" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="290">
@@ -3235,7 +3275,7 @@
         <v>300</v>
       </c>
       <c r="B290" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="291">
@@ -3251,7 +3291,7 @@
         <v>302</v>
       </c>
       <c r="B292" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="293">
@@ -3259,16 +3299,14 @@
         <v>303</v>
       </c>
       <c r="B293" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="s">
         <v>304</v>
       </c>
-      <c r="B294" t="s">
-        <v>13</v>
-      </c>
+      <c r="B294"/>
     </row>
     <row r="295">
       <c r="A295" t="s">
@@ -3281,7 +3319,7 @@
         <v>306</v>
       </c>
       <c r="B296" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="297">
@@ -3289,27 +3327,31 @@
         <v>307</v>
       </c>
       <c r="B297" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="s">
         <v>308</v>
       </c>
-      <c r="B298"/>
+      <c r="B298" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="s">
         <v>309</v>
       </c>
-      <c r="B299"/>
+      <c r="B299" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
         <v>310</v>
       </c>
       <c r="B300" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="301">
@@ -3317,7 +3359,7 @@
         <v>311</v>
       </c>
       <c r="B301" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>